<commit_message>
Feature/redescente lrm hub (#112)
Ajout du cas d'usage de redescente des données de RDV vers les LRM 716be51fa29ab0d1977ee79c13b52f075cd3a5b7
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-FrAppointmentSAS.xlsx
+++ b/main/ig/StructureDefinition-FrAppointmentSAS.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-09T16:27:22+00:00</t>
+    <t>2025-11-04T10:04:56+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -8495,7 +8495,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="66" hidden="true">
+    <row r="66">
       <c r="A66" t="s" s="2">
         <v>398</v>
       </c>
@@ -11763,12 +11763,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AJ97">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>